<commit_message>
Add a TC for valid login
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/invalidLogincredentials.xlsx
+++ b/src/main/resources/testData/invalidLogincredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielslechta/Developer/Selenium/PortfolioProject/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB6182E-E880-5847-A357-A681526C22F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98B99BF-62A6-774C-A08D-B63097A2A427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,16 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>john.smith@test.com</t>
-  </si>
-  <si>
-    <t>lucy.jones@test.com</t>
-  </si>
-  <si>
-    <t>martin.brian@test.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>test123</t>
   </si>
@@ -52,10 +43,16 @@
     <t> </t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>adam1</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
   </si>
 </sst>
 </file>
@@ -99,9 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -396,47 +396,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2">
+        <v>4445555</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>